<commit_message>
Total max power implemented
The way it will work, is that for each point we'll compute what the equivalent rated power to reach that power would be. This is done thanks to surrogate which compute the equivalent thermodynamic power and then a constant ratio between thermodynamc power and rated power is computed.
</commit_message>
<xml_diff>
--- a/src/fastga_he/models/propulsion/components/source/turboshaft/methodology/data_pt6_family.xlsx
+++ b/src/fastga_he/models/propulsion/components/source/turboshaft/methodology/data_pt6_family.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fl.lutz\FAST\FAST-OAD\FAST-OAD-CS23-HE\src\fastga_he\models\propulsion\components\source\turboshaft\methodology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA68FCB-AAFF-4D92-B1C6-AE40DACDE45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907D1993-7AA0-401B-86AC-9A30F0175C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -448,11 +448,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -460,8 +457,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14187,9 +14187,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M77" sqref="M77"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14222,40 +14222,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13" t="s">
+      <c r="I1" s="12"/>
+      <c r="J1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
       <c r="O1" t="s">
         <v>26</v>
       </c>
       <c r="P1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
       <c r="Y1" s="1"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -14334,16 +14334,16 @@
       <c r="Y2" t="s">
         <v>81</v>
       </c>
-      <c r="AA2" s="11" t="s">
+      <c r="AA2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="12"/>
+      <c r="AB2" s="15"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C3">
@@ -14362,10 +14362,10 @@
         <f>F3/$F$4*$G$4</f>
         <v>749.2810734463277</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>30</v>
       </c>
       <c r="J3">
@@ -14413,7 +14413,7 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="11"/>
       <c r="C4">
         <v>1572</v>
       </c>
@@ -14429,8 +14429,8 @@
       <c r="G4">
         <v>474.5</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
       <c r="J4">
         <v>1900</v>
       </c>
@@ -14492,7 +14492,7 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="11"/>
       <c r="C5">
         <v>1572</v>
       </c>
@@ -14509,8 +14509,8 @@
         <f>F5/$F$4*$G$4</f>
         <v>499.96751412429381</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
       <c r="J5">
         <v>1900</v>
       </c>
@@ -14570,7 +14570,7 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="11"/>
       <c r="C6">
         <v>1572</v>
       </c>
@@ -14587,8 +14587,8 @@
         <f t="shared" ref="G6:G44" si="6">F6/$F$4*$G$4</f>
         <v>599.15677966101691</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
       <c r="J6">
         <v>1900</v>
       </c>
@@ -14648,7 +14648,7 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="11"/>
       <c r="C7">
         <v>1341</v>
       </c>
@@ -14665,8 +14665,8 @@
         <f t="shared" si="6"/>
         <v>674.2189265536723</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
       <c r="J7">
         <v>1900</v>
       </c>
@@ -14725,7 +14725,7 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="11"/>
       <c r="C8">
         <v>1572</v>
       </c>
@@ -14742,8 +14742,8 @@
         <f t="shared" si="6"/>
         <v>615.24152542372883</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
       <c r="J8">
         <v>1900</v>
       </c>
@@ -14792,16 +14792,16 @@
         <f t="shared" si="3"/>
         <v>366.61983050847442</v>
       </c>
-      <c r="AA8" s="11" t="s">
+      <c r="AA8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="AB8" s="12"/>
+      <c r="AB8" s="15"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="11"/>
       <c r="C9">
         <v>1572</v>
       </c>
@@ -14818,8 +14818,8 @@
         <f t="shared" si="6"/>
         <v>749.2810734463277</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
       <c r="J9">
         <v>1900</v>
       </c>
@@ -14882,7 +14882,7 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="11"/>
       <c r="C10">
         <v>1572</v>
       </c>
@@ -14899,8 +14899,8 @@
         <f t="shared" si="6"/>
         <v>749.2810734463277</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
       <c r="J10">
         <v>1900</v>
       </c>
@@ -14965,7 +14965,7 @@
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="11"/>
       <c r="C11">
         <v>1629</v>
       </c>
@@ -14982,8 +14982,8 @@
         <f t="shared" si="6"/>
         <v>867.23587570621476</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
       <c r="J11">
         <v>1900</v>
       </c>
@@ -15037,7 +15037,7 @@
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="11"/>
       <c r="C12">
         <v>1629</v>
       </c>
@@ -15054,8 +15054,8 @@
         <f t="shared" si="6"/>
         <v>899.40536723163837</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
       <c r="J12">
         <v>1900</v>
       </c>
@@ -15109,7 +15109,7 @@
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="11"/>
       <c r="C13">
         <v>1629</v>
       </c>
@@ -15126,8 +15126,8 @@
         <f t="shared" si="6"/>
         <v>867.23587570621476</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
       <c r="J13">
         <v>1900</v>
       </c>
@@ -15183,7 +15183,7 @@
       <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C14">
@@ -15202,10 +15202,10 @@
         <f t="shared" si="6"/>
         <v>849.81073446327684</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="13" t="s">
         <v>44</v>
       </c>
       <c r="J14">
@@ -15252,16 +15252,16 @@
         <f t="shared" si="3"/>
         <v>614.01688135593224</v>
       </c>
-      <c r="AA14" s="11" t="s">
+      <c r="AA14" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="AB14" s="12"/>
+      <c r="AB14" s="15"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="15"/>
+      <c r="B15" s="11"/>
       <c r="C15">
         <v>1688</v>
       </c>
@@ -15278,8 +15278,8 @@
         <f t="shared" si="6"/>
         <v>849.81073446327684</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
       <c r="J15">
         <v>2000</v>
       </c>
@@ -15338,7 +15338,7 @@
       <c r="A16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="11"/>
       <c r="C16">
         <v>1688</v>
       </c>
@@ -15355,8 +15355,8 @@
         <f t="shared" si="6"/>
         <v>849.81073446327684</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
       <c r="J16">
         <v>2000</v>
       </c>
@@ -15414,7 +15414,7 @@
       <c r="A17" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="15"/>
+      <c r="B17" s="11"/>
       <c r="C17">
         <v>1845</v>
       </c>
@@ -15431,8 +15431,8 @@
         <f t="shared" si="6"/>
         <v>1018.7005649717515</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
       <c r="J17">
         <v>1700</v>
       </c>
@@ -15491,7 +15491,7 @@
       <c r="A18" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="15"/>
+      <c r="B18" s="11"/>
       <c r="C18">
         <v>1845</v>
       </c>
@@ -15508,8 +15508,8 @@
         <f t="shared" si="6"/>
         <v>1020.0409604519773</v>
       </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
       <c r="J18">
         <v>1700</v>
       </c>
@@ -15568,7 +15568,7 @@
       <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="15"/>
+      <c r="B19" s="11"/>
       <c r="C19">
         <v>1845</v>
       </c>
@@ -15585,8 +15585,8 @@
         <f t="shared" si="6"/>
         <v>1018.7005649717515</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
       <c r="J19">
         <v>1700</v>
       </c>
@@ -15647,7 +15647,7 @@
       <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="15"/>
+      <c r="B20" s="11"/>
       <c r="C20">
         <v>1696</v>
       </c>
@@ -15664,8 +15664,8 @@
         <f t="shared" si="6"/>
         <v>849.81073446327684</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
       <c r="J20">
         <v>2000</v>
       </c>
@@ -15709,7 +15709,7 @@
       <c r="A21" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="15"/>
+      <c r="B21" s="11"/>
       <c r="C21">
         <v>1831</v>
       </c>
@@ -15726,8 +15726,8 @@
         <f t="shared" si="6"/>
         <v>1049.5296610169491</v>
       </c>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
       <c r="J21">
         <v>1700</v>
       </c>
@@ -15780,7 +15780,7 @@
       <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="15"/>
+      <c r="B22" s="11"/>
       <c r="C22">
         <v>1696</v>
       </c>
@@ -15797,8 +15797,8 @@
         <f t="shared" si="6"/>
         <v>849.81073446327684</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
       <c r="J22">
         <v>2000</v>
       </c>
@@ -15845,7 +15845,7 @@
       <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="15"/>
+      <c r="B23" s="11"/>
       <c r="C23">
         <v>1770</v>
       </c>
@@ -15862,8 +15862,8 @@
         <f t="shared" si="6"/>
         <v>949</v>
       </c>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
       <c r="J23">
         <v>2000</v>
       </c>
@@ -15913,7 +15913,7 @@
       <c r="A24" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="15"/>
+      <c r="B24" s="11"/>
       <c r="C24">
         <v>1900</v>
       </c>
@@ -15930,8 +15930,8 @@
         <f t="shared" si="6"/>
         <v>1219.7598870056497</v>
       </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
       <c r="J24">
         <v>1700</v>
       </c>
@@ -15984,7 +15984,7 @@
       <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="15"/>
+      <c r="B25" s="11"/>
       <c r="C25">
         <v>1900</v>
       </c>
@@ -16001,8 +16001,8 @@
         <f t="shared" si="6"/>
         <v>1219.7598870056497</v>
       </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
       <c r="J25">
         <v>1700</v>
       </c>
@@ -16055,7 +16055,7 @@
       <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="15"/>
+      <c r="B26" s="11"/>
       <c r="C26">
         <v>1900</v>
       </c>
@@ -16072,8 +16072,8 @@
         <f t="shared" si="6"/>
         <v>1172.8460451977401</v>
       </c>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
       <c r="J26">
         <v>1700</v>
       </c>
@@ -16126,7 +16126,7 @@
       <c r="A27" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="15"/>
+      <c r="B27" s="11"/>
       <c r="C27">
         <v>1870</v>
       </c>
@@ -16143,8 +16143,8 @@
         <f t="shared" si="6"/>
         <v>1109.8474576271187</v>
       </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
       <c r="J27">
         <v>1700</v>
       </c>
@@ -16191,7 +16191,7 @@
       <c r="A28" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="11" t="s">
         <v>66</v>
       </c>
       <c r="C28" s="4">
@@ -16210,10 +16210,10 @@
         <f t="shared" si="6"/>
         <v>1199.6539548022599</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="13" t="s">
         <v>68</v>
       </c>
       <c r="J28">
@@ -16269,7 +16269,7 @@
       <c r="A29" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="4">
         <v>1888.5</v>
       </c>
@@ -16286,8 +16286,8 @@
         <f t="shared" si="6"/>
         <v>1199.6539548022599</v>
       </c>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
       <c r="J29">
         <v>1700</v>
       </c>
@@ -16341,7 +16341,7 @@
       <c r="A30" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="15"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="4">
         <v>1888.5</v>
       </c>
@@ -16358,8 +16358,8 @@
         <f t="shared" si="6"/>
         <v>1199.6539548022599</v>
       </c>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
       <c r="J30">
         <v>1700</v>
       </c>
@@ -16419,7 +16419,7 @@
       <c r="A31" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="4">
         <v>1913.1</v>
       </c>
@@ -16436,8 +16436,8 @@
         <f t="shared" si="6"/>
         <v>1214.3983050847457</v>
       </c>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
       <c r="J31">
         <v>1700</v>
       </c>
@@ -16494,7 +16494,7 @@
       <c r="A32" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="15"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="4">
         <v>1921.5</v>
       </c>
@@ -16511,8 +16511,8 @@
         <f t="shared" si="6"/>
         <v>1219.7598870056497</v>
       </c>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
       <c r="J32">
         <v>1700</v>
       </c>
@@ -16566,7 +16566,7 @@
       <c r="A33" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="15"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="4">
         <v>1767.3</v>
       </c>
@@ -16583,8 +16583,8 @@
         <f t="shared" si="6"/>
         <v>1219.7598870056497</v>
       </c>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
       <c r="J33">
         <v>1700</v>
       </c>
@@ -16632,7 +16632,7 @@
       <c r="A34" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="15"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="4">
         <v>1921.5</v>
       </c>
@@ -16649,8 +16649,8 @@
         <f t="shared" si="6"/>
         <v>1219.7598870056497</v>
       </c>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
       <c r="J34">
         <v>1700</v>
       </c>
@@ -16701,7 +16701,7 @@
       <c r="A35" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="15"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="4">
         <v>1888.5</v>
       </c>
@@ -16718,8 +16718,8 @@
         <f t="shared" si="6"/>
         <v>1219.7598870056497</v>
       </c>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
       <c r="J35">
         <v>1700</v>
       </c>
@@ -16773,7 +16773,7 @@
       <c r="A36" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="4">
         <v>1921.5</v>
       </c>
@@ -16790,8 +16790,8 @@
         <f t="shared" si="6"/>
         <v>699.68644067796617</v>
       </c>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
       <c r="J36">
         <v>2000</v>
       </c>
@@ -16851,7 +16851,7 @@
       <c r="A37" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="15"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="4">
         <v>1777</v>
       </c>
@@ -16868,8 +16868,8 @@
         <f t="shared" si="6"/>
         <v>849.81073446327684</v>
       </c>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
       <c r="J37">
         <v>2000</v>
       </c>
@@ -16929,7 +16929,7 @@
       <c r="A38" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="15"/>
+      <c r="B38" s="11"/>
       <c r="C38" s="4">
         <v>1913.1</v>
       </c>
@@ -16946,8 +16946,8 @@
         <f t="shared" si="6"/>
         <v>1199.6539548022599</v>
       </c>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
       <c r="J38">
         <v>2000</v>
       </c>
@@ -16998,7 +16998,7 @@
       <c r="A39" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="15"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="4">
         <v>1777</v>
       </c>
@@ -17015,8 +17015,8 @@
         <f t="shared" si="6"/>
         <v>849.81073446327684</v>
       </c>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
       <c r="J39">
         <v>2000</v>
       </c>
@@ -17067,7 +17067,7 @@
       <c r="A40" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="15"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="4">
         <v>1771.7</v>
       </c>
@@ -17084,8 +17084,8 @@
         <f t="shared" si="6"/>
         <v>950.34039548022611</v>
       </c>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
       <c r="J40">
         <v>2000</v>
       </c>
@@ -17133,7 +17133,7 @@
       <c r="A41" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="15"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="4">
         <v>1913.1</v>
       </c>
@@ -17150,8 +17150,8 @@
         <f t="shared" si="6"/>
         <v>1699.6214689265537</v>
       </c>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
       <c r="J41">
         <v>1700</v>
       </c>
@@ -17202,7 +17202,7 @@
       <c r="A42" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="15"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="4">
         <v>1921.5</v>
       </c>
@@ -17219,8 +17219,8 @@
         <f t="shared" si="6"/>
         <v>1199.6539548022599</v>
       </c>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
       <c r="J42">
         <v>1700</v>
       </c>
@@ -17436,6 +17436,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="Q1:X1"/>
+    <mergeCell ref="H28:H42"/>
+    <mergeCell ref="I28:I42"/>
     <mergeCell ref="B28:B42"/>
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="I3:I13"/>
@@ -17446,12 +17452,6 @@
     <mergeCell ref="H14:H27"/>
     <mergeCell ref="I14:I27"/>
     <mergeCell ref="C1:G1"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="Q1:X1"/>
-    <mergeCell ref="H28:H42"/>
-    <mergeCell ref="I28:I42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>